<commit_message>
RAM - write problems
can write bytes, but if comments are removed cannot write correctly
</commit_message>
<xml_diff>
--- a/memory convents with numbers.xlsx
+++ b/memory convents with numbers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9570" windowHeight="6975"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="9570" windowHeight="6975"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -373,7 +373,7 @@
   <dimension ref="A1:B256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E250" sqref="E250"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>